<commit_message>
Update DB and SWP-document
</commit_message>
<xml_diff>
--- a/SWP-document/SWP391-AppDevProject_Backlog-FBS.xlsx
+++ b/SWP-document/SWP391-AppDevProject_Backlog-FBS.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mieG2dCSLjzsfWNZjEnb/UX83E0kQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhuiSGg1zGgCm3daVlj1eDrFXxfEQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="118">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -106,6 +106,12 @@
     <t>Reset password</t>
   </si>
   <si>
+    <t>Iteration 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change password </t>
+  </si>
+  <si>
     <t>View admin page</t>
   </si>
   <si>
@@ -124,13 +130,10 @@
     <t>Search account</t>
   </si>
   <si>
-    <t>Iteration 3</t>
-  </si>
-  <si>
     <t>Update account</t>
   </si>
   <si>
-    <t>Update status Field</t>
+    <t>Update Field</t>
   </si>
   <si>
     <t>Manage list of fields</t>
@@ -142,12 +145,24 @@
     <t>Nguyễn Đức Nhân</t>
   </si>
   <si>
+    <t>View information detail of Field</t>
+  </si>
+  <si>
+    <t>Manage owner’s field detail</t>
+  </si>
+  <si>
     <t>Search Field</t>
   </si>
   <si>
     <t>Delete Field</t>
   </si>
   <si>
+    <t>Create information of new Field</t>
+  </si>
+  <si>
+    <t>Create new field</t>
+  </si>
+  <si>
     <t>Search info history Booking field</t>
   </si>
   <si>
@@ -160,52 +175,43 @@
     <t>Trần Minh Quân</t>
   </si>
   <si>
-    <t>Detail info history booking</t>
-  </si>
-  <si>
-    <t>View Screen Customer</t>
-  </si>
-  <si>
-    <t>View Screen customer</t>
-  </si>
-  <si>
-    <t>Search Active Field</t>
-  </si>
-  <si>
-    <t>View list of field</t>
-  </si>
-  <si>
-    <t>View detail of Field</t>
+    <t>View detail info history booking</t>
+  </si>
+  <si>
+    <t>Update booked field of owner's field</t>
+  </si>
+  <si>
+    <t>View booking history of owner’s field</t>
+  </si>
+  <si>
+    <t>Delete booked field of owner's field</t>
+  </si>
+  <si>
+    <t>View income of all order</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>View Similar Field</t>
   </si>
   <si>
     <t>View field detail</t>
   </si>
   <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>View Similar Field</t>
-  </si>
-  <si>
     <t>Võ  Trung Quân</t>
   </si>
   <si>
-    <t>Update Order Field</t>
+    <t>View Booking Field of customer</t>
   </si>
   <si>
     <t>Booking field</t>
   </si>
   <si>
-    <t xml:space="preserve">Trần Hữu Phúc </t>
-  </si>
-  <si>
-    <t>Delete Order Field</t>
-  </si>
-  <si>
-    <t>Create information Order Field</t>
-  </si>
-  <si>
-    <t>Booking confirm</t>
+    <t>Update Booking Field of customer</t>
+  </si>
+  <si>
+    <t>Delete Booking Field of customer</t>
   </si>
   <si>
     <t>View QR code</t>
@@ -220,121 +226,151 @@
     <t>Check out</t>
   </si>
   <si>
-    <t>View all Order of customer</t>
+    <t>View all booking history of customer</t>
   </si>
   <si>
     <t>View history of booking</t>
   </si>
   <si>
-    <t>Search order of customer</t>
-  </si>
-  <si>
-    <t>View detail booked fields</t>
+    <t>Search booking history of customer</t>
+  </si>
+  <si>
+    <t>View detail booked fields of customer</t>
   </si>
   <si>
     <t>View detail history of booking</t>
   </si>
   <si>
-    <t>View list field of Manager</t>
-  </si>
-  <si>
-    <t>Manage list owner’s field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lê Hoàng Phúc </t>
-  </si>
-  <si>
-    <t>Search field of manager</t>
-  </si>
-  <si>
-    <t>Sort Field of manager</t>
-  </si>
-  <si>
-    <t>Delete Field of manager</t>
-  </si>
-  <si>
-    <t>Create information of new Field</t>
-  </si>
-  <si>
-    <t>Create new field</t>
-  </si>
-  <si>
-    <t>View information detail of Field</t>
-  </si>
-  <si>
-    <t>Manage owner’s field detail</t>
-  </si>
-  <si>
-    <t>View all booking field of customer</t>
-  </si>
-  <si>
-    <t>View booking history of owner’s field</t>
-  </si>
-  <si>
-    <t>Nguyễn  Đức Nhân</t>
-  </si>
-  <si>
-    <t>Search booked Field</t>
-  </si>
-  <si>
-    <t>Delete Customer Booking</t>
-  </si>
-  <si>
-    <t>Final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">View detail booking </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search order </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manage order </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete Order </t>
-  </si>
-  <si>
-    <t>Income of all order</t>
-  </si>
-  <si>
-    <t>Search Food</t>
+    <t>Search food</t>
   </si>
   <si>
     <t>Manage food</t>
   </si>
   <si>
-    <t>Delete Food</t>
-  </si>
-  <si>
-    <t>View Food</t>
-  </si>
-  <si>
-    <t>Update Food</t>
-  </si>
-  <si>
-    <t>Create Food</t>
+    <t>Delete food</t>
+  </si>
+  <si>
+    <t>Manage food detail</t>
+  </si>
+  <si>
+    <t>View food detail</t>
+  </si>
+  <si>
+    <t>Update food</t>
+  </si>
+  <si>
+    <t>Create food</t>
+  </si>
+  <si>
+    <t>Create new foods</t>
   </si>
   <si>
     <t>Create slot of field</t>
   </si>
   <si>
+    <t>Create new slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update slot of field </t>
+  </si>
+  <si>
     <t>Manage slot of Field</t>
   </si>
   <si>
-    <t xml:space="preserve">Update slot of field </t>
-  </si>
-  <si>
     <t>Delete slot of field</t>
   </si>
   <si>
     <t>Search slot of field</t>
   </si>
   <si>
-    <t xml:space="preserve">Change password </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manage account </t>
+    <t>Create category of field</t>
+  </si>
+  <si>
+    <t>Create field category</t>
+  </si>
+  <si>
+    <t>Search category of field</t>
+  </si>
+  <si>
+    <t>Manage field category</t>
+  </si>
+  <si>
+    <t>Delete category of field</t>
+  </si>
+  <si>
+    <t>Update category of field</t>
+  </si>
+  <si>
+    <t>Create category of food</t>
+  </si>
+  <si>
+    <t>Create food category</t>
+  </si>
+  <si>
+    <t>Search category of food</t>
+  </si>
+  <si>
+    <t>Manage food category</t>
+  </si>
+  <si>
+    <t>Delete category of food</t>
+  </si>
+  <si>
+    <t>Update category of food</t>
+  </si>
+  <si>
+    <t>Create role</t>
+  </si>
+  <si>
+    <t>Create new role</t>
+  </si>
+  <si>
+    <t>Search role</t>
+  </si>
+  <si>
+    <t>Manage role</t>
+  </si>
+  <si>
+    <t>Delete role</t>
+  </si>
+  <si>
+    <t>Update role</t>
+  </si>
+  <si>
+    <t>Create city</t>
+  </si>
+  <si>
+    <t>Create new city</t>
+  </si>
+  <si>
+    <t>Search city</t>
+  </si>
+  <si>
+    <t>Manage city</t>
+  </si>
+  <si>
+    <t>Delete city</t>
+  </si>
+  <si>
+    <t>Update city</t>
+  </si>
+  <si>
+    <t>Create location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new location </t>
+  </si>
+  <si>
+    <t>Search location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage location </t>
+  </si>
+  <si>
+    <t>Delete location</t>
+  </si>
+  <si>
+    <t>Update location</t>
   </si>
 </sst>
 </file>
@@ -401,9 +437,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -426,7 +461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -448,6 +483,17 @@
       </top>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -459,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -508,26 +554,49 @@
     <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -775,7 +844,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0" outlineLevelCol="1"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="3.43"/>
-    <col customWidth="1" min="2" max="2" width="39.43" outlineLevel="1"/>
+    <col customWidth="1" min="2" max="2" width="40.86" outlineLevel="1"/>
     <col customWidth="1" min="3" max="3" width="39.0" outlineLevel="1"/>
     <col customWidth="1" min="4" max="4" width="12.86"/>
     <col customWidth="1" min="5" max="5" width="15.29"/>
@@ -1024,56 +1093,56 @@
         <v>24</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8">
         <v>8.0</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>14</v>
+      <c r="B16" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8">
         <v>9.0</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>30</v>
+      <c r="B17" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>33</v>
+      <c r="F17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>14</v>
@@ -1083,49 +1152,49 @@
       <c r="A18" s="8">
         <v>10.0</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>34</v>
+      <c r="B18" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8">
         <v>11.0</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="24" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>10</v>
+        <v>33</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>14</v>
@@ -1135,23 +1204,23 @@
       <c r="A20" s="8">
         <v>12.0</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>40</v>
+      <c r="F20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>14</v>
@@ -1162,22 +1231,22 @@
         <v>13.0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>14</v>
@@ -1190,23 +1259,23 @@
       <c r="B22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>38</v>
+      <c r="C22" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="12" t="s">
+      <c r="E22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>40</v>
       </c>
+      <c r="G22" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="H22" s="13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23">
@@ -1214,10 +1283,10 @@
         <v>15.0</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="19" t="s">
         <v>44</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>22</v>
@@ -1226,13 +1295,13 @@
         <v>11</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
@@ -1240,25 +1309,25 @@
         <v>16.0</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -1266,25 +1335,25 @@
         <v>17.0</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26">
@@ -1292,25 +1361,25 @@
         <v>18.0</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="G26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="H26" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27">
@@ -1320,23 +1389,23 @@
       <c r="B27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="C27" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28">
@@ -1344,25 +1413,25 @@
         <v>20.0</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>53</v>
-      </c>
       <c r="D28" s="12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29">
@@ -1373,48 +1442,48 @@
         <v>55</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8">
         <v>22.0</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="31">
@@ -1422,10 +1491,10 @@
         <v>23.0</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>10</v>
@@ -1434,13 +1503,13 @@
         <v>14</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32">
@@ -1451,22 +1520,22 @@
         <v>61</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>59</v>
+      <c r="F32" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33">
@@ -1474,25 +1543,25 @@
         <v>25.0</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>58</v>
-      </c>
       <c r="D33" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>24</v>
+      <c r="F33" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34">
@@ -1500,25 +1569,25 @@
         <v>26.0</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>13</v>
+      <c r="F34" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35">
@@ -1526,15 +1595,15 @@
         <v>27.0</v>
       </c>
       <c r="B35" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="13" t="s">
+      <c r="D35" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="12" t="s">
@@ -1544,7 +1613,7 @@
         <v>13</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36">
@@ -1552,10 +1621,10 @@
         <v>28.0</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="22" t="s">
         <v>68</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>10</v>
@@ -1563,14 +1632,14 @@
       <c r="E36" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>46</v>
+      <c r="F36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37">
@@ -1580,8 +1649,8 @@
       <c r="B37" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>68</v>
+      <c r="C37" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>10</v>
@@ -1590,13 +1659,13 @@
         <v>14</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38">
@@ -1604,10 +1673,10 @@
         <v>30.0</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="28" t="s">
         <v>70</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>10</v>
@@ -1615,14 +1684,14 @@
       <c r="E38" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>46</v>
+      <c r="F38" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39">
@@ -1638,17 +1707,17 @@
       <c r="D39" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40">
@@ -1656,25 +1725,25 @@
         <v>32.0</v>
       </c>
       <c r="B40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>14</v>
+      <c r="D40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41">
@@ -1684,23 +1753,23 @@
       <c r="B41" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>14</v>
+      <c r="C41" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42">
@@ -1708,84 +1777,84 @@
         <v>34.0</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="8">
         <v>35.0</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>78</v>
+      <c r="B43" s="30" t="s">
+        <v>79</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="8">
         <v>36.0</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="30" t="s">
         <v>80</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="8">
         <v>37.0</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="30" t="s">
         <v>82</v>
       </c>
       <c r="C45" s="16" t="s">
@@ -1795,371 +1864,371 @@
         <v>10</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="8">
         <v>38.0</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="D46" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="8">
         <v>39.0</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="16" t="s">
-        <v>83</v>
+      <c r="C47" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="8">
         <v>40.0</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>83</v>
+      <c r="B48" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>85</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="8">
         <v>41.0</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="16" t="s">
-        <v>90</v>
-      </c>
       <c r="D49" s="12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="8">
         <v>42.0</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="16" t="s">
-        <v>90</v>
-      </c>
       <c r="D50" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="8">
         <v>43.0</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="30" t="s">
         <v>92</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="8">
         <v>44.0</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="30" t="s">
         <v>93</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="8">
         <v>45.0</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="20" t="s">
-        <v>94</v>
-      </c>
       <c r="D53" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F53" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="H53" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="8">
         <v>46.0</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="30" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E54" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="H54" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="8">
         <v>47.0</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="16" t="s">
-        <v>94</v>
-      </c>
       <c r="D55" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E55" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G55" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F55" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="H55" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="8">
         <v>48.0</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>98</v>
+      <c r="B56" s="30" t="s">
+        <v>99</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G56" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F56" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="H56" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="8">
         <v>49.0</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>99</v>
+      <c r="B57" s="30" t="s">
+        <v>100</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="8">
         <v>50.0</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>100</v>
+      <c r="B58" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="8">
         <v>51.0</v>
       </c>
-      <c r="B59" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>100</v>
+      <c r="B59" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>12</v>
@@ -2168,24 +2237,24 @@
         <v>13</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="8">
         <v>52.0</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C60" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C60" s="24" t="s">
-        <v>100</v>
-      </c>
       <c r="D60" s="12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>12</v>
@@ -2194,74 +2263,217 @@
         <v>13</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="8">
         <v>53.0</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>104</v>
+      <c r="B61" s="30" t="s">
+        <v>106</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="25"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
+      <c r="A62" s="8">
+        <v>54.0</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="25"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
+      <c r="A63" s="8">
+        <v>55.0</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="25"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-    </row>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
+      <c r="A64" s="8">
+        <v>56.0</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="A65" s="8">
+        <v>57.0</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="A66" s="8">
+        <v>58.0</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="8">
+        <v>59.0</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="A68" s="8">
+        <v>60.0</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="69" ht="15.75" customHeight="1"/>
     <row r="70" ht="15.75" customHeight="1"/>
     <row r="71" ht="15.75" customHeight="1"/>
@@ -3238,16 +3450,15 @@
     <row r="1042" ht="15.75" customHeight="1"/>
     <row r="1043" ht="15.75" customHeight="1"/>
     <row r="1044" ht="15.75" customHeight="1"/>
-    <row r="1045" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H61">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H68">
       <formula1>"Iteration 1,Iteration 2,Iteration 3,Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D9:D61">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D9:D68">
       <formula1>"Simple,Medium,Complex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E9:E61">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E9:E68">
       <formula1>"Iteration 1,Iteration 2,Iteration 3"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>